<commit_message>
Refactor Python namespace & cleanup (#6)
</commit_message>
<xml_diff>
--- a/tests/data/df.xlsx
+++ b/tests/data/df.xlsx
@@ -434,19 +434,24 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>c</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -459,7 +464,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +477,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="inlineStr">

</xml_diff>